<commit_message>
extra sheet was removed
</commit_message>
<xml_diff>
--- a/suppl_data/SupplData4 - all adpA genes from Streptomyces.xlsx
+++ b/suppl_data/SupplData4 - all adpA genes from Streptomyces.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/_my/github/article-tta-codon/suppl_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72687698-32D9-A74C-902E-B11193D2944C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB657EA-B9CB-3348-BCCD-732747401A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="18040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="18040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
-    <sheet name="Streptomyces_orgs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="767">
   <si>
     <t>CTG</t>
   </si>
@@ -2327,9 +2326,6 @@
   </si>
   <si>
     <t>GTG</t>
-  </si>
-  <si>
-    <t>num_adpA</t>
   </si>
 </sst>
 </file>
@@ -2764,8 +2760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1122F73-9385-2C41-8BD3-33720025B5A8}">
   <dimension ref="A1:K223"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10594,2298 +10590,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C206"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>634</v>
-      </c>
-      <c r="B2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>734</v>
-      </c>
-      <c r="B3" t="s">
-        <v>483</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>722</v>
-      </c>
-      <c r="B4" t="s">
-        <v>450</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>574</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>564</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>567</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>584</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>619</v>
-      </c>
-      <c r="B9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>599</v>
-      </c>
-      <c r="B10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>650</v>
-      </c>
-      <c r="B11" t="s">
-        <v>268</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>640</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>684</v>
-      </c>
-      <c r="B13" t="s">
-        <v>353</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>756</v>
-      </c>
-      <c r="B14" t="s">
-        <v>544</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>719</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>691</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>728</v>
-      </c>
-      <c r="B17" t="s">
-        <v>466</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>733</v>
-      </c>
-      <c r="B18" t="s">
-        <v>480</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>741</v>
-      </c>
-      <c r="B19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>735</v>
-      </c>
-      <c r="B20" t="s">
-        <v>487</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>731</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>750</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>753</v>
-      </c>
-      <c r="B23" t="s">
-        <v>536</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>736</v>
-      </c>
-      <c r="B24" t="s">
-        <v>490</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>749</v>
-      </c>
-      <c r="B25" t="s">
-        <v>280</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>642</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>739</v>
-      </c>
-      <c r="B27" t="s">
-        <v>499</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>720</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>565</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>723</v>
-      </c>
-      <c r="B30" t="s">
-        <v>454</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>740</v>
-      </c>
-      <c r="B31" t="s">
-        <v>502</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>663</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>717</v>
-      </c>
-      <c r="B33" t="s">
-        <v>437</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>745</v>
-      </c>
-      <c r="B34" t="s">
-        <v>265</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>751</v>
-      </c>
-      <c r="B35" t="s">
-        <v>530</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>738</v>
-      </c>
-      <c r="B36" t="s">
-        <v>496</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>755</v>
-      </c>
-      <c r="B37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>752</v>
-      </c>
-      <c r="B38" t="s">
-        <v>533</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>573</v>
-      </c>
-      <c r="B39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>557</v>
-      </c>
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>732</v>
-      </c>
-      <c r="B41" t="s">
-        <v>477</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>747</v>
-      </c>
-      <c r="B42" t="s">
-        <v>521</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>558</v>
-      </c>
-      <c r="B43" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>742</v>
-      </c>
-      <c r="B44" t="s">
-        <v>507</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>560</v>
-      </c>
-      <c r="B45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>561</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>553</v>
-      </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
-        <v>554</v>
-      </c>
-      <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
-        <v>556</v>
-      </c>
-      <c r="B49" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
-        <v>754</v>
-      </c>
-      <c r="B50" t="s">
-        <v>539</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
-        <v>744</v>
-      </c>
-      <c r="B51" t="s">
-        <v>513</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>570</v>
-      </c>
-      <c r="B52" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
-        <v>572</v>
-      </c>
-      <c r="B53" t="s">
-        <v>54</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
-        <v>757</v>
-      </c>
-      <c r="B54" t="s">
-        <v>174</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
-        <v>575</v>
-      </c>
-      <c r="B55" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
-        <v>563</v>
-      </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
-        <v>571</v>
-      </c>
-      <c r="B57" t="s">
-        <v>51</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
-        <v>559</v>
-      </c>
-      <c r="B58" t="s">
-        <v>18</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
-        <v>566</v>
-      </c>
-      <c r="B59" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60" t="s">
-        <v>562</v>
-      </c>
-      <c r="B60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
-        <v>585</v>
-      </c>
-      <c r="B61" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A62" t="s">
-        <v>711</v>
-      </c>
-      <c r="B62" t="s">
-        <v>365</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
-        <v>588</v>
-      </c>
-      <c r="B63" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
-        <v>743</v>
-      </c>
-      <c r="B64" t="s">
-        <v>510</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
-        <v>586</v>
-      </c>
-      <c r="B65" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
-        <v>569</v>
-      </c>
-      <c r="B66" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A67" t="s">
-        <v>578</v>
-      </c>
-      <c r="B67" t="s">
-        <v>71</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A68" t="s">
-        <v>580</v>
-      </c>
-      <c r="B68" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" t="s">
-        <v>746</v>
-      </c>
-      <c r="B69" t="s">
-        <v>518</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A70" t="s">
-        <v>610</v>
-      </c>
-      <c r="B70" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A71" t="s">
-        <v>613</v>
-      </c>
-      <c r="B71" t="s">
-        <v>169</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A72" t="s">
-        <v>612</v>
-      </c>
-      <c r="B72" t="s">
-        <v>166</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A73" t="s">
-        <v>621</v>
-      </c>
-      <c r="B73" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A74" t="s">
-        <v>625</v>
-      </c>
-      <c r="B74" t="s">
-        <v>196</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A75" t="s">
-        <v>626</v>
-      </c>
-      <c r="B75" t="s">
-        <v>199</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A76" t="s">
-        <v>555</v>
-      </c>
-      <c r="B76" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A77" t="s">
-        <v>576</v>
-      </c>
-      <c r="B77" t="s">
-        <v>66</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A78" t="s">
-        <v>577</v>
-      </c>
-      <c r="B78" t="s">
-        <v>6</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79" t="s">
-        <v>579</v>
-      </c>
-      <c r="B79" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80" t="s">
-        <v>628</v>
-      </c>
-      <c r="B80" t="s">
-        <v>205</v>
-      </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A81" t="s">
-        <v>627</v>
-      </c>
-      <c r="B81" t="s">
-        <v>202</v>
-      </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A82" t="s">
-        <v>631</v>
-      </c>
-      <c r="B82" t="s">
-        <v>214</v>
-      </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A83" t="s">
-        <v>604</v>
-      </c>
-      <c r="B83" t="s">
-        <v>144</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A84" t="s">
-        <v>606</v>
-      </c>
-      <c r="B84" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A85" t="s">
-        <v>630</v>
-      </c>
-      <c r="B85" t="s">
-        <v>211</v>
-      </c>
-      <c r="C85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A86" t="s">
-        <v>587</v>
-      </c>
-      <c r="B86" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A87" t="s">
-        <v>607</v>
-      </c>
-      <c r="B87" t="s">
-        <v>152</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A88" t="s">
-        <v>629</v>
-      </c>
-      <c r="B88" t="s">
-        <v>208</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A89" t="s">
-        <v>608</v>
-      </c>
-      <c r="B89" t="s">
-        <v>155</v>
-      </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A90" t="s">
-        <v>624</v>
-      </c>
-      <c r="B90" t="s">
-        <v>6</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A91" t="s">
-        <v>622</v>
-      </c>
-      <c r="B91" t="s">
-        <v>6</v>
-      </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A92" t="s">
-        <v>623</v>
-      </c>
-      <c r="B92" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A93" t="s">
-        <v>635</v>
-      </c>
-      <c r="B93" t="s">
-        <v>227</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A94" t="s">
-        <v>636</v>
-      </c>
-      <c r="B94" t="s">
-        <v>230</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A95" t="s">
-        <v>609</v>
-      </c>
-      <c r="B95" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A96" t="s">
-        <v>605</v>
-      </c>
-      <c r="B96" t="s">
-        <v>147</v>
-      </c>
-      <c r="C96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A97" t="s">
-        <v>632</v>
-      </c>
-      <c r="B97" t="s">
-        <v>6</v>
-      </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A98" t="s">
-        <v>611</v>
-      </c>
-      <c r="B98" t="s">
-        <v>163</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A99" t="s">
-        <v>581</v>
-      </c>
-      <c r="B99" t="s">
-        <v>6</v>
-      </c>
-      <c r="C99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A100" t="s">
-        <v>582</v>
-      </c>
-      <c r="B100" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A101" t="s">
-        <v>602</v>
-      </c>
-      <c r="B101" t="s">
-        <v>139</v>
-      </c>
-      <c r="C101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A102" t="s">
-        <v>583</v>
-      </c>
-      <c r="B102" t="s">
-        <v>83</v>
-      </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A103" t="s">
-        <v>646</v>
-      </c>
-      <c r="B103" t="s">
-        <v>6</v>
-      </c>
-      <c r="C103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A104" t="s">
-        <v>648</v>
-      </c>
-      <c r="B104" t="s">
-        <v>262</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A105" t="s">
-        <v>641</v>
-      </c>
-      <c r="B105" t="s">
-        <v>244</v>
-      </c>
-      <c r="C105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A106" t="s">
-        <v>620</v>
-      </c>
-      <c r="B106" t="s">
-        <v>174</v>
-      </c>
-      <c r="C106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A107" t="s">
-        <v>617</v>
-      </c>
-      <c r="B107" t="s">
-        <v>174</v>
-      </c>
-      <c r="C107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A108" t="s">
-        <v>618</v>
-      </c>
-      <c r="B108" t="s">
-        <v>174</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A109" t="s">
-        <v>616</v>
-      </c>
-      <c r="B109" t="s">
-        <v>174</v>
-      </c>
-      <c r="C109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A110" t="s">
-        <v>615</v>
-      </c>
-      <c r="B110" t="s">
-        <v>174</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A111" t="s">
-        <v>595</v>
-      </c>
-      <c r="B111" t="s">
-        <v>118</v>
-      </c>
-      <c r="C111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A112" t="s">
-        <v>594</v>
-      </c>
-      <c r="B112" t="s">
-        <v>115</v>
-      </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A113" t="s">
-        <v>593</v>
-      </c>
-      <c r="B113" t="s">
-        <v>112</v>
-      </c>
-      <c r="C113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A114" t="s">
-        <v>592</v>
-      </c>
-      <c r="B114" t="s">
-        <v>109</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A115" t="s">
-        <v>591</v>
-      </c>
-      <c r="B115" t="s">
-        <v>106</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A116" t="s">
-        <v>590</v>
-      </c>
-      <c r="B116" t="s">
-        <v>103</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A117" t="s">
-        <v>589</v>
-      </c>
-      <c r="B117" t="s">
-        <v>100</v>
-      </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A118" t="s">
-        <v>600</v>
-      </c>
-      <c r="B118" t="s">
-        <v>134</v>
-      </c>
-      <c r="C118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A119" t="s">
-        <v>598</v>
-      </c>
-      <c r="B119" t="s">
-        <v>127</v>
-      </c>
-      <c r="C119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A120" t="s">
-        <v>596</v>
-      </c>
-      <c r="B120" t="s">
-        <v>121</v>
-      </c>
-      <c r="C120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A121" t="s">
-        <v>647</v>
-      </c>
-      <c r="B121" t="s">
-        <v>259</v>
-      </c>
-      <c r="C121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A122" t="s">
-        <v>644</v>
-      </c>
-      <c r="B122" t="s">
-        <v>6</v>
-      </c>
-      <c r="C122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A123" t="s">
-        <v>643</v>
-      </c>
-      <c r="B123" t="s">
-        <v>249</v>
-      </c>
-      <c r="C123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A124" t="s">
-        <v>654</v>
-      </c>
-      <c r="B124" t="s">
-        <v>280</v>
-      </c>
-      <c r="C124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A125" t="s">
-        <v>597</v>
-      </c>
-      <c r="B125" t="s">
-        <v>124</v>
-      </c>
-      <c r="C125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A126" t="s">
-        <v>655</v>
-      </c>
-      <c r="B126" t="s">
-        <v>6</v>
-      </c>
-      <c r="C126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A127" t="s">
-        <v>656</v>
-      </c>
-      <c r="B127" t="s">
-        <v>285</v>
-      </c>
-      <c r="C127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A128" t="s">
-        <v>657</v>
-      </c>
-      <c r="B128" t="s">
-        <v>6</v>
-      </c>
-      <c r="C128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A129" t="s">
-        <v>633</v>
-      </c>
-      <c r="B129" t="s">
-        <v>219</v>
-      </c>
-      <c r="C129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A130" t="s">
-        <v>658</v>
-      </c>
-      <c r="B130" t="s">
-        <v>6</v>
-      </c>
-      <c r="C130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A131" t="s">
-        <v>660</v>
-      </c>
-      <c r="B131" t="s">
-        <v>6</v>
-      </c>
-      <c r="C131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A132" t="s">
-        <v>659</v>
-      </c>
-      <c r="B132" t="s">
-        <v>6</v>
-      </c>
-      <c r="C132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A133" t="s">
-        <v>661</v>
-      </c>
-      <c r="B133" t="s">
-        <v>6</v>
-      </c>
-      <c r="C133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A134" t="s">
-        <v>614</v>
-      </c>
-      <c r="B134" t="s">
-        <v>6</v>
-      </c>
-      <c r="C134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A135" t="s">
-        <v>748</v>
-      </c>
-      <c r="B135" t="s">
-        <v>6</v>
-      </c>
-      <c r="C135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A136" t="s">
-        <v>649</v>
-      </c>
-      <c r="B136" t="s">
-        <v>265</v>
-      </c>
-      <c r="C136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A137" t="s">
-        <v>652</v>
-      </c>
-      <c r="B137" t="s">
-        <v>6</v>
-      </c>
-      <c r="C137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A138" t="s">
-        <v>637</v>
-      </c>
-      <c r="B138" t="s">
-        <v>6</v>
-      </c>
-      <c r="C138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A139" t="s">
-        <v>665</v>
-      </c>
-      <c r="B139" t="s">
-        <v>305</v>
-      </c>
-      <c r="C139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A140" t="s">
-        <v>662</v>
-      </c>
-      <c r="B140" t="s">
-        <v>6</v>
-      </c>
-      <c r="C140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A141" t="s">
-        <v>669</v>
-      </c>
-      <c r="B141" t="s">
-        <v>6</v>
-      </c>
-      <c r="C141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A142" t="s">
-        <v>670</v>
-      </c>
-      <c r="B142" t="s">
-        <v>6</v>
-      </c>
-      <c r="C142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A143" t="s">
-        <v>671</v>
-      </c>
-      <c r="B143" t="s">
-        <v>6</v>
-      </c>
-      <c r="C143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A144" t="s">
-        <v>653</v>
-      </c>
-      <c r="B144" t="s">
-        <v>277</v>
-      </c>
-      <c r="C144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A145" t="s">
-        <v>676</v>
-      </c>
-      <c r="B145" t="s">
-        <v>6</v>
-      </c>
-      <c r="C145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A146" t="s">
-        <v>674</v>
-      </c>
-      <c r="B146" t="s">
-        <v>6</v>
-      </c>
-      <c r="C146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A147" t="s">
-        <v>675</v>
-      </c>
-      <c r="B147" t="s">
-        <v>6</v>
-      </c>
-      <c r="C147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A148" t="s">
-        <v>673</v>
-      </c>
-      <c r="B148" t="s">
-        <v>324</v>
-      </c>
-      <c r="C148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A149" t="s">
-        <v>672</v>
-      </c>
-      <c r="B149" t="s">
-        <v>321</v>
-      </c>
-      <c r="C149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A150" t="s">
-        <v>645</v>
-      </c>
-      <c r="B150" t="s">
-        <v>254</v>
-      </c>
-      <c r="C150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A151" t="s">
-        <v>677</v>
-      </c>
-      <c r="B151" t="s">
-        <v>6</v>
-      </c>
-      <c r="C151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A152" t="s">
-        <v>638</v>
-      </c>
-      <c r="B152" t="s">
-        <v>235</v>
-      </c>
-      <c r="C152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A153" t="s">
-        <v>639</v>
-      </c>
-      <c r="B153" t="s">
-        <v>238</v>
-      </c>
-      <c r="C153">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A154" t="s">
-        <v>681</v>
-      </c>
-      <c r="B154" t="s">
-        <v>344</v>
-      </c>
-      <c r="C154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A155" t="s">
-        <v>682</v>
-      </c>
-      <c r="B155" t="s">
-        <v>347</v>
-      </c>
-      <c r="C155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A156" t="s">
-        <v>680</v>
-      </c>
-      <c r="B156" t="s">
-        <v>341</v>
-      </c>
-      <c r="C156">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A157" t="s">
-        <v>668</v>
-      </c>
-      <c r="B157" t="s">
-        <v>312</v>
-      </c>
-      <c r="C157">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A158" t="s">
-        <v>683</v>
-      </c>
-      <c r="B158" t="s">
-        <v>350</v>
-      </c>
-      <c r="C158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A159" t="s">
-        <v>686</v>
-      </c>
-      <c r="B159" t="s">
-        <v>359</v>
-      </c>
-      <c r="C159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A160" t="s">
-        <v>664</v>
-      </c>
-      <c r="B160" t="s">
-        <v>302</v>
-      </c>
-      <c r="C160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A161" t="s">
-        <v>651</v>
-      </c>
-      <c r="B161" t="s">
-        <v>272</v>
-      </c>
-      <c r="C161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A162" t="s">
-        <v>679</v>
-      </c>
-      <c r="B162" t="s">
-        <v>338</v>
-      </c>
-      <c r="C162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A163" t="s">
-        <v>690</v>
-      </c>
-      <c r="B163" t="s">
-        <v>371</v>
-      </c>
-      <c r="C163">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A164" t="s">
-        <v>678</v>
-      </c>
-      <c r="B164" t="s">
-        <v>335</v>
-      </c>
-      <c r="C164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A165" t="s">
-        <v>687</v>
-      </c>
-      <c r="B165" t="s">
-        <v>362</v>
-      </c>
-      <c r="C165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A166" t="s">
-        <v>730</v>
-      </c>
-      <c r="B166" t="s">
-        <v>472</v>
-      </c>
-      <c r="C166">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A167" t="s">
-        <v>694</v>
-      </c>
-      <c r="B167" t="s">
-        <v>381</v>
-      </c>
-      <c r="C167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A168" t="s">
-        <v>689</v>
-      </c>
-      <c r="B168" t="s">
-        <v>368</v>
-      </c>
-      <c r="C168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A169" t="s">
-        <v>685</v>
-      </c>
-      <c r="B169" t="s">
-        <v>6</v>
-      </c>
-      <c r="C169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A170" t="s">
-        <v>704</v>
-      </c>
-      <c r="B170" t="s">
-        <v>6</v>
-      </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A171" t="s">
-        <v>707</v>
-      </c>
-      <c r="B171" t="s">
-        <v>6</v>
-      </c>
-      <c r="C171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A172" t="s">
-        <v>709</v>
-      </c>
-      <c r="B172" t="s">
-        <v>6</v>
-      </c>
-      <c r="C172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A173" t="s">
-        <v>710</v>
-      </c>
-      <c r="B173" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A174" t="s">
-        <v>712</v>
-      </c>
-      <c r="B174" t="s">
-        <v>423</v>
-      </c>
-      <c r="C174">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A175" t="s">
-        <v>695</v>
-      </c>
-      <c r="B175" t="s">
-        <v>384</v>
-      </c>
-      <c r="C175">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A176" t="s">
-        <v>698</v>
-      </c>
-      <c r="B176" t="s">
-        <v>6</v>
-      </c>
-      <c r="C176">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A177" t="s">
-        <v>696</v>
-      </c>
-      <c r="B177" t="s">
-        <v>6</v>
-      </c>
-      <c r="C177">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A178" t="s">
-        <v>700</v>
-      </c>
-      <c r="B178" t="s">
-        <v>396</v>
-      </c>
-      <c r="C178">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A179" t="s">
-        <v>699</v>
-      </c>
-      <c r="B179" t="s">
-        <v>393</v>
-      </c>
-      <c r="C179">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A180" t="s">
-        <v>708</v>
-      </c>
-      <c r="B180" t="s">
-        <v>6</v>
-      </c>
-      <c r="C180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A181" t="s">
-        <v>701</v>
-      </c>
-      <c r="B181" t="s">
-        <v>399</v>
-      </c>
-      <c r="C181">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A182" t="s">
-        <v>715</v>
-      </c>
-      <c r="B182" t="s">
-        <v>6</v>
-      </c>
-      <c r="C182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A183" t="s">
-        <v>714</v>
-      </c>
-      <c r="B183" t="s">
-        <v>429</v>
-      </c>
-      <c r="C183">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A184" t="s">
-        <v>716</v>
-      </c>
-      <c r="B184" t="s">
-        <v>434</v>
-      </c>
-      <c r="C184">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A185" t="s">
-        <v>697</v>
-      </c>
-      <c r="B185" t="s">
-        <v>6</v>
-      </c>
-      <c r="C185">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A186" t="s">
-        <v>703</v>
-      </c>
-      <c r="B186" t="s">
-        <v>6</v>
-      </c>
-      <c r="C186">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A187" t="s">
-        <v>718</v>
-      </c>
-      <c r="B187" t="s">
-        <v>6</v>
-      </c>
-      <c r="C187">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A188" t="s">
-        <v>603</v>
-      </c>
-      <c r="B188" t="s">
-        <v>6</v>
-      </c>
-      <c r="C188">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A189" t="s">
-        <v>706</v>
-      </c>
-      <c r="B189" t="s">
-        <v>410</v>
-      </c>
-      <c r="C189">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A190" t="s">
-        <v>713</v>
-      </c>
-      <c r="B190" t="s">
-        <v>426</v>
-      </c>
-      <c r="C190">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A191" t="s">
-        <v>688</v>
-      </c>
-      <c r="B191" t="s">
-        <v>365</v>
-      </c>
-      <c r="C191">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A192" t="s">
-        <v>705</v>
-      </c>
-      <c r="B192" t="s">
-        <v>6</v>
-      </c>
-      <c r="C192">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A193" t="s">
-        <v>666</v>
-      </c>
-      <c r="B193" t="s">
-        <v>6</v>
-      </c>
-      <c r="C193">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A194" t="s">
-        <v>724</v>
-      </c>
-      <c r="B194" t="s">
-        <v>6</v>
-      </c>
-      <c r="C194">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A195" t="s">
-        <v>667</v>
-      </c>
-      <c r="B195" t="s">
-        <v>147</v>
-      </c>
-      <c r="C195">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A196" t="s">
-        <v>725</v>
-      </c>
-      <c r="B196" t="s">
-        <v>6</v>
-      </c>
-      <c r="C196">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A197" t="s">
-        <v>702</v>
-      </c>
-      <c r="B197" t="s">
-        <v>6</v>
-      </c>
-      <c r="C197">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A198" t="s">
-        <v>721</v>
-      </c>
-      <c r="B198" t="s">
-        <v>447</v>
-      </c>
-      <c r="C198">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A199" t="s">
-        <v>726</v>
-      </c>
-      <c r="B199" t="s">
-        <v>6</v>
-      </c>
-      <c r="C199">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A200" t="s">
-        <v>727</v>
-      </c>
-      <c r="B200" t="s">
-        <v>463</v>
-      </c>
-      <c r="C200">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A201" t="s">
-        <v>729</v>
-      </c>
-      <c r="B201" t="s">
-        <v>6</v>
-      </c>
-      <c r="C201">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A202" t="s">
-        <v>692</v>
-      </c>
-      <c r="B202" t="s">
-        <v>6</v>
-      </c>
-      <c r="C202">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A203" t="s">
-        <v>568</v>
-      </c>
-      <c r="B203" t="s">
-        <v>6</v>
-      </c>
-      <c r="C203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A204" t="s">
-        <v>601</v>
-      </c>
-      <c r="B204" t="s">
-        <v>6</v>
-      </c>
-      <c r="C204">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A205" t="s">
-        <v>737</v>
-      </c>
-      <c r="B205" t="s">
-        <v>493</v>
-      </c>
-      <c r="C205">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A206" t="s">
-        <v>693</v>
-      </c>
-      <c r="B206" t="s">
-        <v>6</v>
-      </c>
-      <c r="C206">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C206">
-    <sortCondition descending="1" ref="C2"/>
-  </sortState>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>